<commit_message>
adding NEI data and data read in
</commit_message>
<xml_diff>
--- a/output/Transitions Rule/summary_tables/transition_rule_summary_tables_APC-Geismar.xlsx
+++ b/output/Transitions Rule/summary_tables/transition_rule_summary_tables_APC-Geismar.xlsx
@@ -1,92 +1,99 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\Git Repos\F_Gas_Rules\output\Transitions Rule\summary_tables\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E76C1A-B245-4DB4-98B1-3E1BA501AA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Means" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Standard Deviations" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Means" sheetId="1" r:id="rId1"/>
+    <sheet name="Standard Deviations" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t xml:space="preserve">Variable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rural Areas (National Average)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rural Areas (State Average)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Within 1 mile of HFC production facility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Within 3 miles of HFC production facility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Within 5 miles of HFC production facility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Within 10 miles of HFC production facility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% White</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Rural Areas (National Average)</t>
+  </si>
+  <si>
+    <t>Rural Areas (State Average)</t>
+  </si>
+  <si>
+    <t>Within 1 mile of HFC production facility</t>
+  </si>
+  <si>
+    <t>Within 3 miles of HFC production facility</t>
+  </si>
+  <si>
+    <t>Within 5 miles of HFC production facility</t>
+  </si>
+  <si>
+    <t>Within 10 miles of HFC production facility</t>
+  </si>
+  <si>
+    <t>% White</t>
   </si>
   <si>
     <t xml:space="preserve">% Black or African American </t>
   </si>
   <si>
-    <t xml:space="preserve">% Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% Hispanic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Median Income [1,000 2019$]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% Below Poverty Line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% Below Half the Poverty Line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Cancer Risk (per million)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Respiratory (hazard quotient)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rural Areas (National Average) SD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rural Areas (State Average) SD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Within 1 mile of HFC production facility SD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Within 3 mile of HFC production facility SD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Within 5 mile of HFC production facility SD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Within 10 mile of HFC production facility SD</t>
+    <t>% Other</t>
+  </si>
+  <si>
+    <t>% Hispanic</t>
+  </si>
+  <si>
+    <t>Median Income [1,000 2019$]</t>
+  </si>
+  <si>
+    <t>% Below Poverty Line</t>
+  </si>
+  <si>
+    <t>% Below Half the Poverty Line</t>
+  </si>
+  <si>
+    <t>Total Cancer Risk (per million)</t>
+  </si>
+  <si>
+    <t>Total Respiratory (hazard quotient)</t>
+  </si>
+  <si>
+    <t>Rural Areas (National Average) SD</t>
+  </si>
+  <si>
+    <t>Rural Areas (State Average) SD</t>
+  </si>
+  <si>
+    <t>Within 1 mile of HFC production facility SD</t>
+  </si>
+  <si>
+    <t>Within 3 mile of HFC production facility SD</t>
+  </si>
+  <si>
+    <t>Within 5 mile of HFC production facility SD</t>
+  </si>
+  <si>
+    <t>Within 10 mile of HFC production facility SD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -115,13 +122,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -403,258 +422,263 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>84</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>70</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>63</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>70</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>56</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>68</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>7.6</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>25</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>30</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>26</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>39</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>27</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="n">
-        <v>8.2</v>
-      </c>
-      <c r="C4" t="n">
+      <c r="B4">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C4">
         <v>4.7</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>6.6</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>4</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>5.3</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>5.7</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>10</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>3.6</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>1.2</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>3.3</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>4.7</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>5</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>67</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>53</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>86</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>83</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>79</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>80</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>6.8</v>
       </c>
-      <c r="C7" t="n">
-        <v>9.8</v>
-      </c>
-      <c r="D7" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="E7" t="n">
+      <c r="C7">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E7">
         <v>3.8</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>6.3</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>5.3</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="n">
-        <v>5.1</v>
-      </c>
-      <c r="C8" t="n">
+      <c r="B8">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C8">
         <v>7.8</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>6.5</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>5.3</v>
       </c>
-      <c r="F8" t="n">
-        <v>8.3</v>
-      </c>
-      <c r="G8" t="n">
+      <c r="F8">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="G8">
         <v>5.4</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>26</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>39</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>93</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>95</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9">
         <v>93</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9">
         <v>81</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>0.32</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>0.43</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>0.5</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>0.5</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10">
         <v>0.51</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10">
         <v>0.5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -677,215 +701,215 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>19</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>28</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>2.7</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>8.9</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>23</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>29</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>16</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>28</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>3.5</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>6.3</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>23</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>29</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>12</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>6.6</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>0.83</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>3.1</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>8.1</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>5.8</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>15</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>5.3</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>2.5</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>16</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>9</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>6.2</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>28</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>21</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>24</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>26</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>34</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>31</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>7.6</v>
       </c>
-      <c r="C7" t="n">
-        <v>9.7</v>
-      </c>
-      <c r="D7" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="E7" t="n">
+      <c r="C7">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="D7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E7">
         <v>2.7</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>7.9</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>7.1</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>6.4</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>8.9</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>12</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>8</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8">
         <v>11</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8">
         <v>8.6</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>8.6</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>24</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>14</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>15</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9">
         <v>32</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9">
         <v>35</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.084</v>
-      </c>
-      <c r="D10" t="n">
+      <c r="B10">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C10">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="D10">
         <v>0</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10" t="n">
-        <v>0.039</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.065</v>
+      <c r="F10">
+        <v>3.9E-2</v>
+      </c>
+      <c r="G10">
+        <v>6.5000000000000002E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>